<commit_message>
fix bugs result double display
</commit_message>
<xml_diff>
--- a/data/template/raw data untuk crosscek pam baru.xlsx
+++ b/data/template/raw data untuk crosscek pam baru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/d_bodro_cifor-icraf_org/Documents/dw/project R/theme 2/lusita/shiny/data/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/d_bodro_cifor-icraf_org/Documents/dw/project R/theme 2/lusita/data/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{C9953028-729E-4230-BDED-2387E9D6C9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F67D9DDD-D9DA-41CF-80F6-09A90E90B319}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{C9953028-729E-4230-BDED-2387E9D6C9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63CEC4AE-E404-49AD-B9E4-3E4B8F0ED5D6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{434F79F2-1D89-4230-B38A-FBCE8A0F0489}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{434F79F2-1D89-4230-B38A-FBCE8A0F0489}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="94">
   <si>
     <t>Urea</t>
   </si>
@@ -200,13 +200,124 @@
     <t>kerja</t>
   </si>
   <si>
-    <t>"tenaga kerja|tk|kerja|tenaga"</t>
-  </si>
-  <si>
     <t>HARUS LOWCASE</t>
   </si>
   <si>
-    <t>"hok|HOK"</t>
+    <t>utama</t>
+  </si>
+  <si>
+    <t>COKLAT AF</t>
+  </si>
+  <si>
+    <t>DUKU AF</t>
+  </si>
+  <si>
+    <t>JATI AF</t>
+  </si>
+  <si>
+    <t>KARET AF</t>
+  </si>
+  <si>
+    <t>KARET AF PADI BUAH</t>
+  </si>
+  <si>
+    <t>KARET AF PADI KOPI</t>
+  </si>
+  <si>
+    <t>KAYU MANIS AF</t>
+  </si>
+  <si>
+    <t>KEBUN CAMPUR AF</t>
+  </si>
+  <si>
+    <t>KELAPA AF</t>
+  </si>
+  <si>
+    <t>KELAPA AF COKLAT</t>
+  </si>
+  <si>
+    <t>KELAPA AF JAGUNG</t>
+  </si>
+  <si>
+    <t>KELAPA SAWIT AF</t>
+  </si>
+  <si>
+    <t>KEMIRI AF</t>
+  </si>
+  <si>
+    <t>KOPI AF</t>
+  </si>
+  <si>
+    <t>LOGGING AF</t>
+  </si>
+  <si>
+    <t>SALAK AF</t>
+  </si>
+  <si>
+    <t>SENGON AF</t>
+  </si>
+  <si>
+    <t>CENGKEH</t>
+  </si>
+  <si>
+    <t>COKLAT</t>
+  </si>
+  <si>
+    <t>JAGUNG</t>
+  </si>
+  <si>
+    <t>JATI</t>
+  </si>
+  <si>
+    <t>KARET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAYU MANIS  </t>
+  </si>
+  <si>
+    <t>KELAPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KELAPA </t>
+  </si>
+  <si>
+    <t>KELAPA SAWIT</t>
+  </si>
+  <si>
+    <t>KELAPA SAWIT LARGE SCALE</t>
+  </si>
+  <si>
+    <t>KENTANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOPI   </t>
+  </si>
+  <si>
+    <t>LADA</t>
+  </si>
+  <si>
+    <t>PADI</t>
+  </si>
+  <si>
+    <t>PADI DRYLAND</t>
+  </si>
+  <si>
+    <t>PADI IRIGASI</t>
+  </si>
+  <si>
+    <t>PADI WETLAND</t>
+  </si>
+  <si>
+    <t>PINANG</t>
+  </si>
+  <si>
+    <t>SAGU</t>
+  </si>
+  <si>
+    <t>SENGON</t>
+  </si>
+  <si>
+    <t>TEH</t>
   </si>
 </sst>
 </file>
@@ -214,8 +325,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -289,11 +400,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,9 +414,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -326,14 +438,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +479,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +585,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +727,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,24 +735,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E76978D-30F8-4CCF-8060-75D8D0F1ED70}">
-  <dimension ref="A1:AG75"/>
+  <dimension ref="A1:AG93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="27" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -660,9 +767,9 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>47</v>
@@ -674,7 +781,7 @@
         <v>7.0199999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E3" s="4" t="s">
         <v>49</v>
       </c>
@@ -685,7 +792,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E4" s="4" t="s">
         <v>50</v>
       </c>
@@ -696,7 +803,7 @@
         <v>14775</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -787,7 +894,7 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -878,7 +985,7 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -969,7 +1076,7 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1060,7 +1167,7 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1151,7 +1258,7 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1242,7 +1349,7 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1333,7 +1440,7 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1424,7 +1531,7 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1515,7 +1622,7 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1606,7 +1713,7 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1697,7 +1804,7 @@
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1788,7 +1895,7 @@
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1879,7 +1986,7 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1970,7 +2077,7 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -2061,7 +2168,7 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -2152,7 +2259,7 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -2243,7 +2350,7 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -2334,7 +2441,7 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2425,7 +2532,7 @@
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -2470,7 +2577,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -2561,7 +2668,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -2652,7 +2759,7 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -2743,7 +2850,7 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -2834,7 +2941,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -2925,7 +3032,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -3016,7 +3123,7 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
@@ -3107,7 +3214,7 @@
       <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>52</v>
       </c>
@@ -3198,7 +3305,7 @@
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3233,15 +3340,15 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
+      <c r="C34" t="s">
+        <v>1</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -3250,381 +3357,468 @@
         <v>0</v>
       </c>
       <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>2658.5160642857145</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>4044.8571428571431</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>4829.469542857144</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>6852.8980928571427</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>8728.8017142857152</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>10457.180407142858</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>12038.034171428573</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>13471.363007142858</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>14757.166914285717</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>15895.445892857144</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>16886.19994285714</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>17729.42906428572</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <v>18425.133257142861</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <v>18973.312521428572</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>19373.966857142863</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>19627.096264285716</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>19732.700742857145</v>
       </c>
-      <c r="W34">
+      <c r="X34">
         <v>19690.780292857147</v>
       </c>
-      <c r="X34">
+      <c r="Y34">
         <v>19501.334914285715</v>
       </c>
-      <c r="Y34">
+      <c r="Z34">
         <v>19164.364607142859</v>
       </c>
-      <c r="Z34">
+      <c r="AA34">
         <v>18679.869371428573</v>
       </c>
-      <c r="AA34">
+      <c r="AB34">
         <v>18047.849207142859</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="10">
         <v>9000</v>
       </c>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D37" s="10">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="10">
         <v>14000</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D38" s="10">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D39" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D40" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="10">
         <v>90000</v>
       </c>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D41" s="10">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="10">
         <v>102000</v>
       </c>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D42" s="10">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="10">
         <v>95000</v>
       </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D43" s="10">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D44" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="10">
         <v>38000</v>
       </c>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D45" s="10">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
       <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="10">
         <v>93000</v>
       </c>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D46" s="10">
+        <v>93000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
       <c r="B47" t="s">
         <v>43</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="10">
         <v>585000</v>
       </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="D47" s="10">
+        <v>585000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
       <c r="B48" t="s">
         <v>43</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="10">
         <v>500000</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="10">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
       <c r="B49" t="s">
         <v>43</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="10">
         <v>460000</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="10">
+        <v>460000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
       <c r="B50" t="s">
         <v>43</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="10">
         <v>80000</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="10">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
       <c r="B51" t="s">
         <v>43</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="10">
         <v>5500000</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="10">
+        <v>5500000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>19</v>
       </c>
       <c r="B52" t="s">
         <v>43</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="10">
         <v>50000</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="10">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>20</v>
       </c>
       <c r="B53" t="s">
         <v>43</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="10">
         <v>300000</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="10">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
       <c r="B54" t="s">
         <v>43</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="10">
         <v>200000</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="10">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
       <c r="B55" t="s">
         <v>43</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>37</v>
       </c>
       <c r="B56" t="s">
         <v>44</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="10">
         <v>30000</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" s="10">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
       <c r="B57" t="s">
         <v>45</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D57" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>25</v>
       </c>
       <c r="B58" t="s">
         <v>45</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D58" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>26</v>
       </c>
       <c r="B59" t="s">
         <v>45</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>27</v>
       </c>
       <c r="B60" t="s">
         <v>45</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>28</v>
       </c>
       <c r="B61" t="s">
         <v>45</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D61" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>29</v>
       </c>
       <c r="B62" t="s">
         <v>45</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D62" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
       <c r="B63" t="s">
         <v>45</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D63" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>31</v>
       </c>
       <c r="B64" t="s">
         <v>45</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -3634,25 +3828,164 @@
       <c r="C66">
         <v>1570</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
+      <c r="D66">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="9">
-        <v>3151000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="9">
-        <v>1830000</v>
+      <c r="D73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="D80" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>68</v>
+      </c>
+      <c r="D85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>69</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>70</v>
+      </c>
+      <c r="D87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>71</v>
+      </c>
+      <c r="D88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>72</v>
+      </c>
+      <c r="D89" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>